<commit_message>
add citation info and links to the dbGAP data inventory
</commit_message>
<xml_diff>
--- a/AML31_DBGAP_Submission_Info.xlsx
+++ b/AML31_DBGAP_Submission_Info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="420" yWindow="0" windowWidth="51120" windowHeight="28000" tabRatio="500"/>
@@ -945,7 +945,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -954,6 +954,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
@@ -1525,12 +1528,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="860" activePane="bottomLeft"/>
-      <selection activeCell="L1" sqref="L1:L1048576"/>
-      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
+      <selection activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1544,10 +1547,11 @@
     <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="18.140625" customWidth="1"/>
-    <col min="11" max="11" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="62.85546875" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -1582,7 +1586,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -1613,11 +1617,12 @@
       <c r="J2" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -1648,11 +1653,11 @@
       <c r="J3" t="s">
         <v>70</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="6" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -1683,11 +1688,11 @@
       <c r="J4" t="s">
         <v>70</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1718,11 +1723,12 @@
       <c r="J5" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="6" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1753,11 +1759,12 @@
       <c r="J6" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="6" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -1788,11 +1795,12 @@
       <c r="J7" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="6" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -1823,11 +1831,12 @@
       <c r="J8" t="s">
         <v>70</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>108</v>
       </c>
@@ -1858,11 +1867,12 @@
       <c r="J9" t="s">
         <v>70</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="6" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>109</v>
       </c>
@@ -1893,11 +1903,12 @@
       <c r="J10" t="s">
         <v>70</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="K10" s="6" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>110</v>
       </c>
@@ -1928,11 +1939,12 @@
       <c r="J11" t="s">
         <v>70</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="6" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -1963,11 +1975,11 @@
       <c r="J12" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="6" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -1998,11 +2010,11 @@
       <c r="J13" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="6" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -2033,11 +2045,11 @@
       <c r="J14" t="s">
         <v>70</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="6" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -2068,11 +2080,11 @@
       <c r="J15" t="s">
         <v>70</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="6" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -2103,11 +2115,11 @@
       <c r="J16" t="s">
         <v>70</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="6" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -2138,11 +2150,11 @@
       <c r="J17" t="s">
         <v>70</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="6" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -2173,11 +2185,11 @@
       <c r="J18" t="s">
         <v>69</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>118</v>
       </c>
@@ -2208,11 +2220,11 @@
       <c r="J19" t="s">
         <v>70</v>
       </c>
-      <c r="K19" s="5" t="s">
+      <c r="K19" s="6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>119</v>
       </c>
@@ -2243,11 +2255,11 @@
       <c r="J20" t="s">
         <v>70</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="6" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>120</v>
       </c>
@@ -2278,11 +2290,12 @@
       <c r="J21" t="s">
         <v>70</v>
       </c>
-      <c r="K21" s="5" t="s">
+      <c r="K21" s="6" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21" s="5"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>121</v>
       </c>
@@ -2313,11 +2326,12 @@
       <c r="J22" t="s">
         <v>70</v>
       </c>
-      <c r="K22" s="5" t="s">
+      <c r="K22" s="6" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>122</v>
       </c>
@@ -2348,11 +2362,12 @@
       <c r="J23" t="s">
         <v>70</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="K23" s="6" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="5"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>123</v>
       </c>
@@ -2383,11 +2398,12 @@
       <c r="J24" t="s">
         <v>70</v>
       </c>
-      <c r="K24" s="5" t="s">
+      <c r="K24" s="6" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24" s="5"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>124</v>
       </c>
@@ -2418,11 +2434,12 @@
       <c r="J25" t="s">
         <v>70</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="6" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25" s="5"/>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>125</v>
       </c>
@@ -2453,11 +2470,12 @@
       <c r="J26" t="s">
         <v>70</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26" s="5"/>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -2488,11 +2506,12 @@
       <c r="J27" t="s">
         <v>70</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="K27" s="6" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27" s="5"/>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -2523,11 +2542,11 @@
       <c r="J28" t="s">
         <v>70</v>
       </c>
-      <c r="K28" s="5" t="s">
+      <c r="K28" s="6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>128</v>
       </c>
@@ -2558,11 +2577,11 @@
       <c r="J29" t="s">
         <v>70</v>
       </c>
-      <c r="K29" s="5" t="s">
+      <c r="K29" s="6" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>129</v>
       </c>
@@ -2593,11 +2612,11 @@
       <c r="J30" t="s">
         <v>70</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="K30" s="6" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:12">
       <c r="A31" t="s">
         <v>130</v>
       </c>
@@ -2628,11 +2647,11 @@
       <c r="J31" t="s">
         <v>70</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="K31" s="6" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>131</v>
       </c>
@@ -2663,11 +2682,11 @@
       <c r="J32" t="s">
         <v>70</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="K32" s="6" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:12">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -2698,11 +2717,11 @@
       <c r="J33" t="s">
         <v>70</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="K33" s="6" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:12">
       <c r="A34" t="s">
         <v>133</v>
       </c>
@@ -2733,11 +2752,11 @@
       <c r="J34" t="s">
         <v>70</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="K34" s="6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:12">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -2768,11 +2787,11 @@
       <c r="J35" t="s">
         <v>70</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="K35" s="6" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:12">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -2803,11 +2822,11 @@
       <c r="J36" t="s">
         <v>70</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K36" s="6" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:12">
       <c r="A37" t="s">
         <v>136</v>
       </c>
@@ -2838,11 +2857,11 @@
       <c r="J37" t="s">
         <v>70</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="6" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:12">
       <c r="A38" t="s">
         <v>137</v>
       </c>
@@ -2873,11 +2892,11 @@
       <c r="J38" t="s">
         <v>69</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="6" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:12">
       <c r="A39" t="s">
         <v>138</v>
       </c>
@@ -2908,11 +2927,11 @@
       <c r="J39" t="s">
         <v>70</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="K39" s="6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:12">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -2943,11 +2962,11 @@
       <c r="J40" t="s">
         <v>70</v>
       </c>
-      <c r="K40" s="5" t="s">
+      <c r="K40" s="6" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:12">
       <c r="A41" t="s">
         <v>140</v>
       </c>
@@ -2978,11 +2997,12 @@
       <c r="J41" t="s">
         <v>70</v>
       </c>
-      <c r="K41" s="5" t="s">
+      <c r="K41" s="6" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42" t="s">
         <v>141</v>
       </c>
@@ -3013,11 +3033,12 @@
       <c r="J42" t="s">
         <v>70</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="K42" s="6" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>142</v>
       </c>
@@ -3048,11 +3069,12 @@
       <c r="J43" t="s">
         <v>70</v>
       </c>
-      <c r="K43" s="5" t="s">
+      <c r="K43" s="6" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43" s="5"/>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44" t="s">
         <v>143</v>
       </c>
@@ -3083,11 +3105,12 @@
       <c r="J44" t="s">
         <v>70</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="K44" s="6" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44" s="5"/>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45" t="s">
         <v>144</v>
       </c>
@@ -3118,11 +3141,12 @@
       <c r="J45" t="s">
         <v>70</v>
       </c>
-      <c r="K45" s="5" t="s">
+      <c r="K45" s="6" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45" s="5"/>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46" t="s">
         <v>145</v>
       </c>
@@ -3153,11 +3177,12 @@
       <c r="J46" t="s">
         <v>70</v>
       </c>
-      <c r="K46" s="5" t="s">
+      <c r="K46" s="6" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -3188,11 +3213,12 @@
       <c r="J47" t="s">
         <v>70</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="K47" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47" s="5"/>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -3223,7 +3249,7 @@
       <c r="J48" t="s">
         <v>70</v>
       </c>
-      <c r="K48" s="5" t="s">
+      <c r="K48" s="6" t="s">
         <v>202</v>
       </c>
     </row>
@@ -3258,7 +3284,7 @@
       <c r="J49" t="s">
         <v>70</v>
       </c>
-      <c r="K49" s="5" t="s">
+      <c r="K49" s="6" t="s">
         <v>203</v>
       </c>
     </row>
@@ -3293,7 +3319,7 @@
       <c r="J50" t="s">
         <v>70</v>
       </c>
-      <c r="K50" s="5" t="s">
+      <c r="K50" s="6" t="s">
         <v>204</v>
       </c>
     </row>
@@ -3328,7 +3354,7 @@
       <c r="J51" t="s">
         <v>70</v>
       </c>
-      <c r="K51" s="5" t="s">
+      <c r="K51" s="6" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3363,7 +3389,7 @@
       <c r="J52" t="s">
         <v>154</v>
       </c>
-      <c r="K52" s="5" t="s">
+      <c r="K52" s="6" t="s">
         <v>206</v>
       </c>
     </row>
@@ -3398,7 +3424,7 @@
       <c r="J53" t="s">
         <v>154</v>
       </c>
-      <c r="K53" s="5" t="s">
+      <c r="K53" s="6" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>